<commit_message>
Updated Framework To Hybrid Mode
</commit_message>
<xml_diff>
--- a/resources-testdata/TestData.xlsx
+++ b/resources-testdata/TestData.xlsx
@@ -3,12 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26815"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED45A0FB-762B-4641-99F0-951B1DBFD1B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{367662E5-20D5-45AC-8D99-F7DE3B94CC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData01" sheetId="1" r:id="rId1"/>
+    <sheet name="TestData02" sheetId="2" r:id="rId2"/>
+    <sheet name="TestData03" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -76,13 +78,31 @@
   </si>
   <si>
     <t>Sauce Labs Bike Light</t>
+  </si>
+  <si>
+    <t>API Positive</t>
+  </si>
+  <si>
+    <t>eve.holt@reqres.in</t>
+  </si>
+  <si>
+    <t>cityslicka</t>
+  </si>
+  <si>
+    <t>API Negative</t>
+  </si>
+  <si>
+    <t>test@gmail.com</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +114,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,18 +177,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -511,4 +542,134 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19134957-B8B8-435E-A1CD-7A708DE601D1}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D51D3904-A93A-4F50-BACB-D351D067C635}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0CE5E07-7BF0-4F25-A63E-C5105DAC70A4}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{BEAF383D-B39E-4F09-96A8-0F57D470F9E9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
 </file>
</xml_diff>